<commit_message>
new work on extractor
</commit_message>
<xml_diff>
--- a/tools/ExtractAWAPdata4locations/zones.xlsx
+++ b/tools/ExtractAWAPdata4locations/zones.xlsx
@@ -17,15 +17,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>zones</t>
   </si>
   <si>
     <t>Kaleen, ACT</t>
-  </si>
-  <si>
-    <t>Scullin, ACT</t>
   </si>
 </sst>
 </file>
@@ -122,11 +119,11 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -139,11 +136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="3">
-      <c r="A3" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="3"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="4"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="5"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="6"/>
@@ -174,7 +167,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9843137254902"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -199,7 +192,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9843137254902"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>